<commit_message>
xlsx edits and pdf corrections + ds files
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb58/raw/Table11.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb58/raw/Table11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/wc_climate_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb58/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DA9261-6E08-7947-A1A1-71AD8CBC2C08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE56E910-EDEF-A344-A63A-ED89AD789DE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
   <si>
     <t>Region of residence</t>
   </si>
@@ -131,7 +131,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -184,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,25 +208,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -544,11 +541,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="29"/>
     <col min="2" max="2" width="31"/>
@@ -570,23 +567,28 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>151</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>32</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -595,41 +597,48 @@
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <v>69</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>229</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>151</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>28</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -638,61 +647,72 @@
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <v>26</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>434</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>479</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>436</v>
       </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A11" s="5"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>298</v>
       </c>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A12" s="5"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>83</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>35</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -701,51 +721,60 @@
       <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>105</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>1436</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>557</v>
       </c>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A16" s="5"/>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>439</v>
       </c>
-      <c r="D16" s="11"/>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A17" s="5"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>77</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>36</v>
       </c>
-      <c r="D18" s="11"/>
+      <c r="D18" s="10"/>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -754,41 +783,48 @@
       <c r="B19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="12">
         <v>86</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <v>1195</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="B20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>308</v>
       </c>
-      <c r="D20" s="11"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>15</v>
       </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
+      <c r="A22" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="B22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>12</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
@@ -797,61 +833,72 @@
       <c r="B23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>58</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="9">
         <v>1815</v>
       </c>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A25" s="5"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>718</v>
       </c>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A26" s="5"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>494</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="10"/>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
+      <c r="A27" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="9">
         <v>206</v>
       </c>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A28" s="5"/>
+      <c r="D27" s="10"/>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28" s="11">
         <v>79</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
@@ -860,61 +907,72 @@
       <c r="B29" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="12">
         <v>222</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="11">
         <v>3534</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="9">
         <v>703</v>
       </c>
-      <c r="D30" s="11"/>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A31" s="5"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B31" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31" s="11">
         <v>264</v>
       </c>
-      <c r="D31" s="11"/>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A32" s="5"/>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="11">
         <v>251</v>
       </c>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A33" s="5"/>
+      <c r="D32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="11">
         <v>152</v>
       </c>
-      <c r="D33" s="11"/>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A34" s="5"/>
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="B34" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="12">
         <v>21</v>
       </c>
-      <c r="D34" s="11"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
@@ -923,41 +981,48 @@
       <c r="B35" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="12">
         <v>61</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="11">
         <v>1452</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="B36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="9">
         <v>148</v>
       </c>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A37" s="8"/>
+      <c r="D36" s="10"/>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="B37" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="11">
         <v>146</v>
       </c>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.15">
-      <c r="A38" s="5"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="B38" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38" s="11">
         <v>38</v>
       </c>
-      <c r="D38" s="11"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
@@ -966,29 +1031,29 @@
       <c r="B39" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39" s="11">
         <v>19</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="11">
         <v>351</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.15">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="5"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="13">
+      <c r="C40" s="10"/>
+      <c r="D40" s="12">
         <v>9047</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="14" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="14" t="s">
+    <row r="41" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15">
+      <c r="C41" s="14"/>
+      <c r="D41" s="14">
         <f>SUM(D2:D39)-D40</f>
         <v>0</v>
       </c>

</xml_diff>